<commit_message>
generated EML for full data package however Validation failed
</commit_message>
<xml_diff>
--- a/level1b_test.xlsx
+++ b/level1b_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="6" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>NaN</t>
   </si>
   <si>
-    <t>permalink</t>
-  </si>
-  <si>
     <t>data_provider_category_HumanObservation</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
     <t>eventID</t>
   </si>
   <si>
-    <t>Unique URL identifier pointing to the landing page for the ROI in an external repository. This is used to generate the eventID and occurrenceID</t>
-  </si>
-  <si>
     <t>Darwin Core unique identifier for the sample as an Event (http://rs.tdwg.org/dwc/terms/eventID)</t>
   </si>
   <si>
@@ -223,6 +217,12 @@
   </si>
   <si>
     <t>taxon that can not be classified under any of the 3 listed higher level phytoplankton groups</t>
+  </si>
+  <si>
+    <t>associatedMedia</t>
+  </si>
+  <si>
+    <t>Unique URL identifier pointing to the landing page for the ROI in an external repository. Darwin Core term http://rs.tdwg.org/dwc/terms/associatedMedia. This is used to generate the occurrenceID.</t>
   </si>
 </sst>
 </file>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,12 +580,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -599,10 +599,10 @@
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -616,67 +616,67 @@
     </row>
     <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
         <v>44</v>
-      </c>
-      <c r="G4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
         <v>44</v>
-      </c>
-      <c r="G5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
         <v>44</v>
-      </c>
-      <c r="G6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
@@ -687,16 +687,16 @@
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
@@ -707,16 +707,16 @@
     </row>
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
@@ -727,16 +727,16 @@
     </row>
     <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
@@ -747,16 +747,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
@@ -767,10 +767,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -787,10 +787,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -827,10 +827,10 @@
     </row>
     <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -844,10 +844,10 @@
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -861,10 +861,10 @@
     </row>
     <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -878,10 +878,10 @@
     </row>
     <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -903,7 +903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD5"/>
     </sheetView>
   </sheetViews>
@@ -911,57 +911,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
         <v>55</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>